<commit_message>
meta data for cohorts 1 and 2 now permanently combined
</commit_message>
<xml_diff>
--- a/Cohort1/MetaData/MelanomaCohort1_CellTypes.xlsx
+++ b/Cohort1/MetaData/MelanomaCohort1_CellTypes.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\HaloData\Melanoma_IL2__Final\Cohort1\MetaData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4CEE6D4A-D040-430C-BA6D-FBE2D599ADAE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="4365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple" sheetId="1" r:id="rId1"/>
     <sheet name="Complex" sheetId="2" r:id="rId2"/>
+    <sheet name="Other" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t>Marker_combination</t>
   </si>
@@ -87,68 +89,212 @@
     <t>Natural killer cell</t>
   </si>
   <si>
-    <t>Macrophage</t>
-  </si>
-  <si>
     <t>T cell</t>
   </si>
   <si>
     <t>Subtype</t>
   </si>
   <si>
+    <t>IF</t>
+  </si>
+  <si>
+    <t>OF</t>
+  </si>
+  <si>
+    <t>MATCHES</t>
+  </si>
+  <si>
+    <t>CELL_TYPE</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>CD4,CD14,CD163,CD68</t>
+  </si>
+  <si>
+    <t>CD3,CD56</t>
+  </si>
+  <si>
+    <t>Negatives</t>
+  </si>
+  <si>
+    <t>With_OR_Without</t>
+  </si>
+  <si>
+    <t>CD3,CD8,CD56</t>
+  </si>
+  <si>
+    <t>NEGATIVES</t>
+  </si>
+  <si>
+    <t>SUBTYPE</t>
+  </si>
+  <si>
+    <t>CD14,CD163,CD68</t>
+  </si>
+  <si>
+    <t>CD8-,FOXP3-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD4-,FOXP3-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD8-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD4-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD4-,CD8-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD3-,CD8-,FOXP3-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD8-,FOXP3-,CD20-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD3-,CD8-,FOXP3-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>Natural killer T cell/CD8</t>
+  </si>
+  <si>
+    <t>CD3,CD4,CD56</t>
+  </si>
+  <si>
+    <t>Natural killer T cell/CD4</t>
+  </si>
+  <si>
+    <t>CD4-,FOXP3-,CD20-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD4-,CD8-,FOXP3-,CD20-,SOX10-</t>
+  </si>
+  <si>
+    <t>S100B</t>
+  </si>
+  <si>
+    <t>Adipocyte or dendritic cell (Langerhans)</t>
+  </si>
+  <si>
+    <t>CD56,S100B</t>
+  </si>
+  <si>
+    <t>Nerve</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Tconv4</t>
+  </si>
+  <si>
+    <t>Tconv8</t>
+  </si>
+  <si>
+    <t>Treg</t>
+  </si>
+  <si>
+    <t>Treg4</t>
+  </si>
+  <si>
+    <t>Treg8</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>NK</t>
+  </si>
+  <si>
+    <t>NKT</t>
+  </si>
+  <si>
+    <t>NKT8</t>
+  </si>
+  <si>
+    <t>NKT4</t>
+  </si>
+  <si>
+    <t>CD3-,CD4-,CD8-,FOXP3-,CD20-,SOX10-,S100B-</t>
+  </si>
+  <si>
+    <t>CD3-,CD4-,CD8-,FOXP3-,CD20-,CD56-,CD14-,CD163-,CD68-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD3-,CD4-,CD8-,FOXP3-,CD20-,CD14-,CD163-,CD68-,SOX10-</t>
+  </si>
+  <si>
+    <t>Macrophage/monocyte</t>
+  </si>
+  <si>
     <t>CD3</t>
   </si>
   <si>
-    <t>SOX10,FOXP3</t>
-  </si>
-  <si>
-    <t>SOX10,CD56</t>
-  </si>
-  <si>
-    <t>IF</t>
-  </si>
-  <si>
-    <t>OF</t>
-  </si>
-  <si>
-    <t>MATCHES</t>
-  </si>
-  <si>
-    <t>CELL_TYPE</t>
-  </si>
-  <si>
-    <t>ANY</t>
-  </si>
-  <si>
-    <t>CD4,CD14,CD163,CD68</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
-    <t>&lt;0.03</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>&lt;=2</t>
+    <t>CD4-,CD8-,FOXP3-,CD20-,CD56-,SOX10-</t>
   </si>
   <si>
     <t>T cell/null phenotype</t>
   </si>
   <si>
+    <t>Tnull</t>
+  </si>
+  <si>
     <t>CD3,CD4,CD8</t>
   </si>
   <si>
-    <t>CD3,CD56</t>
+    <t>FOXP3-,CD20-,CD56-,SOX10-</t>
+  </si>
+  <si>
+    <t>CD4+/CD8+ T cell</t>
+  </si>
+  <si>
+    <t>T4_8</t>
+  </si>
+  <si>
+    <t>Macrophage_monocyte</t>
+  </si>
+  <si>
+    <t>CD3-,CD4-,CD8-,FOXP3-,CD20-</t>
+  </si>
+  <si>
+    <t>CD14,CD163,CD68,CD56</t>
+  </si>
+  <si>
+    <t>CD68,MHCII</t>
+  </si>
+  <si>
+    <t>CD163,MHCII</t>
+  </si>
+  <si>
+    <t>CD68</t>
+  </si>
+  <si>
+    <t>CD163</t>
+  </si>
+  <si>
+    <t>CD3-,CD8-,FOXP3-,CD20-,CD56-,SOX10-, MHCII-</t>
+  </si>
+  <si>
+    <t>CD163,CD14,CD4</t>
+  </si>
+  <si>
+    <t>CD68,CD14,CD4</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,14 +314,6 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,12 +347,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -534,159 +670,326 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="72.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E14" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="F14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -701,91 +1004,205 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="22" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="2"/>
+    <col min="4" max="4" width="20.85546875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>10</v>
+      <c r="E2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF80127D-332C-4A3D-873C-BE6C9045D88C}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>